<commit_message>
ToString и excel-report у BranchedTask
</commit_message>
<xml_diff>
--- a/TaskMaster/newreport.xlsx
+++ b/TaskMaster/newreport.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Topic</t>
   </si>
@@ -39,7 +39,7 @@
     <t>Owner</t>
   </si>
   <si>
-    <t>myTopic</t>
+    <t>chech</t>
   </si>
   <si>
     <t>myDesckription</t>
@@ -58,6 +58,18 @@
   </si>
   <si>
     <t>Valera</t>
+  </si>
+  <si>
+    <t>nya</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>InProcess</t>
+  </si>
+  <si>
+    <t>SubTasks</t>
   </si>
 </sst>
 </file>
@@ -103,7 +115,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -161,6 +173,23 @@
         <v>14</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <headerFooter/>
 </worksheet>
@@ -168,11 +197,62 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>